<commit_message>
finally done with the code block data
</commit_message>
<xml_diff>
--- a/src/scripts/CodeBlocks/code blocks.xlsx
+++ b/src/scripts/CodeBlocks/code blocks.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin of the Lake\workspace\Repos\FrontEndCapstone\src\scripts\CodeBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FCEECC-C3FC-41C8-BC80-727F7FA4F9A7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7462C33F-4AFC-4F1C-9F3D-E2040D0673EE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="9285" xr2:uid="{CB3B7D12-EE88-4088-ADA6-0AA53F93C8FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$50</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="257">
   <si>
     <t>blockID</t>
   </si>
@@ -792,6 +795,440 @@
     <t>git create branch branchName</t>
   </si>
   <si>
+    <t>If Condition</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for (let i = 0; i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCF433E"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>= 100; i++) {\n string += a\n}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for (___ i = 0; i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCF433E"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>= 100; i__) {\n string += a\n}</t>
+    </r>
+  </si>
+  <si>
+    <t>while (vet i = 0; i = 100; i--) {\n string += a\n}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">for (let i = 0; i </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCF433E"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>= 100; i++) {Æ string += aÆ}</t>
+    </r>
+  </si>
+  <si>
+    <t>For Loop</t>
+  </si>
+  <si>
+    <t>ForEach Loop</t>
+  </si>
+  <si>
+    <t>const conjunction = (firstWord, secondWord) =&gt; {\n return `${firstWord} ${secondWord}`\n}\nconsole.log(conjunction(\'Master\', \'Card\'))</t>
+  </si>
+  <si>
+    <t>_____ conjunction = (firstWord, secondWord) __ {\n return ___firstWord} ${secondWord}`\n}\nconsole.___(___________(\'Master\', \'Card\'))</t>
+  </si>
+  <si>
+    <t>const conjunction = (\'firstWord\', \'secondWord\') : {\n return `\'firstWord\' 'secondWord'`\n}\nxbox.console(conjunction(\'Master\', \'Card\'))</t>
+  </si>
+  <si>
+    <t>const conjunction = (firstWord, secondWord) =&gt; {Æ return `${firstWord} ${secondWord}`Æ}Æconsole.log(conjunction(\'Master\', \'Card\'))</t>
+  </si>
+  <si>
+    <t>Interpolation</t>
+  </si>
+  <si>
+    <t>nav ul li {\n display: inline;\n padding: 2em;\n}</t>
+  </si>
+  <si>
+    <t>nav ul li _\n display: inline;\n padding: 2__;\n}</t>
+  </si>
+  <si>
+    <t>nav ul li (\n show: online;\n space-around: 2em;\n)</t>
+  </si>
+  <si>
+    <t>nav ul li {Æ display: inline;Æ padding: 2em;Æ}</t>
+  </si>
+  <si>
+    <t>Nested CSS</t>
+  </si>
+  <si>
+    <t>const steve = {\n name: \'Steve Brownlee\',\n job: \'Instructor\'\n}</t>
+  </si>
+  <si>
+    <t>_____ steve _ {\n name_ _Steve Brownlee_,\n ___: \'Instructor\'\n_</t>
+  </si>
+  <si>
+    <t>create steve = [\n name: \'Steve Brownlee\',\n job: \'Rock Star\'\n]</t>
+  </si>
+  <si>
+    <t>const steve = {Æ name: \'Steve Brownlee\',Æ job: \'Instructor\'Æ}</t>
+  </si>
+  <si>
+    <t>Creating Objects</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>const person = Object.create({}, {\n name: {\n value: \'Kimmy Bird\',\n enumerable: true\n },\n job: {\n value: \'Instructor\',\n enumerable: true\n }\n})</t>
+  </si>
+  <si>
+    <t>const person = ______.______(__, {\n name: {\n _____: \'Kimmy Bird\',\n enumerable: ____\n },\n job: {\n value: _Instructor_,\n __________: true\n }\n})</t>
+  </si>
+  <si>
+    <t>create person = Object.spawn({\n name: {\n value: \'Kimmy Bird\',\n enumberable: true\n },\n job: {\n value: \'Code Wizard\',\n enumerable: false\n }\n})</t>
+  </si>
+  <si>
+    <t>const person = Object.create({}, {Æ name: {Æ value: \'Kimmy Bird\',Æ enumerable: trueÆ },Æ job: {Æ value: \'Instructor\',Æ enumerable: trueÆ }Æ})</t>
+  </si>
+  <si>
+    <t>Object.create</t>
+  </si>
+  <si>
+    <t>const capPlanets = planets.map(planet =&gt; {\n return planet.charAt(0).toUpperCase() + planet.slice(1)\n})</t>
+  </si>
+  <si>
+    <t>const capPlanets = planets.___(planet __ {\n ______ planet.charAt(0).toUpperCase() + ______.slice(1)\n})</t>
+  </si>
+  <si>
+    <t>const capPlanets = planets.map((function) planet =&gt; {\n return planet.characterAt(0).toUpper() + planet.lice(1)\n})</t>
+  </si>
+  <si>
+    <t>const capPlanets = planets.map(planet =&gt; {Æ return planet.charAt(0).toUpperCase() + planet.slice(1)Æ})</t>
+  </si>
+  <si>
+    <t>Array Maps</t>
+  </si>
+  <si>
+    <t>const filteredPlanets = planets.filter(planet =&gt; {\n const containsE = planet.includes(\'e\')\n return containsE\n})</t>
+  </si>
+  <si>
+    <t>const filteredPlanets = planets.______(planet =&gt; {\n _____ containsE = planet.includes(\'_\')\n return _________\n})</t>
+  </si>
+  <si>
+    <t>const filteredPlanets = planets.addFilter(planet (function) {\n if containsE = planet.hasCharmander(\'e\')\n provide containsE\n})</t>
+  </si>
+  <si>
+    <t>const filteredPlanets = planets.filter(planet =&gt; {Æ const containsE = planet.includes(\'e\')Æ return containsEÆ})</t>
+  </si>
+  <si>
+    <t>Array Filters</t>
+  </si>
+  <si>
+    <t>const words = [\'an\', \'early\', \'bird\']\nconst sentence = words.reduce(\n   (partial, next) =&gt; partial + \' \' + next\n)</t>
+  </si>
+  <si>
+    <t>const words = _\'an\', \'early\', \'bird\'_\nconst sentence = _____.reduce(\n   (partial, next) __ partial + \' \' + ____\n)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">const words = [an, early, bird]\nconst sentence = words.induce(\n   (partial </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFCF433E"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> next) = partial + \' \' + next\n)</t>
+    </r>
+  </si>
+  <si>
+    <t>const words = [\'an\', \'early\', \'bird\']Æconst sentence = words.reduce(Æ (partial, next) =&gt; partial + \' \' + nextÆ)</t>
+  </si>
+  <si>
+    <t>Array Reduce</t>
+  </si>
+  <si>
+    <t>.top li {\n list-style: none;\n display: inline;\n}</t>
+  </si>
+  <si>
+    <t>.top li {\n list-_____: none;\n _______: inline;\n}</t>
+  </si>
+  <si>
+    <t>.top li {\n list-style: noBullet;\n display: true;\n}</t>
+  </si>
+  <si>
+    <t>.top li {Æ list-style: none;Æ display: inline;Æ}</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>.n-child section:nth-of-type(even){\n border: 1px solid green;\n}</t>
+  </si>
+  <si>
+    <t>.n-child section:___-of-type(even){\n border: ___ solid green;\n}</t>
+  </si>
+  <si>
+    <t>.n-child section:4th-oft-hype(steven){\n border: solid green 1px;\n}</t>
+  </si>
+  <si>
+    <t>.n-child section:nth-of-type(even){Æ border: 1px solid green;Æ}</t>
+  </si>
+  <si>
+    <t>CSS Pseudo Selectors</t>
+  </si>
+  <si>
+    <t>.top li:not(:last-child)::after {\n content: \',\';\n}</t>
+  </si>
+  <si>
+    <t>.top li:___(:____-child)__after {\n content: \',\';\n}</t>
+  </si>
+  <si>
+    <t>.top li:not(:last-parent)::while {\n content: \';\n}</t>
+  </si>
+  <si>
+    <t>.top li:not(:last-child)::after {Æ content: \',\';Æ}</t>
+  </si>
+  <si>
+    <t>const customers = {\n "location": {\n "city": "Crystal"\n },\n "last_name": "Weimann",\n "job": {\n "position": "Future Web Representative"\n },\n "first_name": "Brittany",\n "contacts": {\n "mobile": "1-327-084-4643",\n "email": [\n "recusandae23@outlook.com"\n ]\n }\n}</t>
+  </si>
+  <si>
+    <t>_____ customers = {\n "location": {\n _city_: "Crystal"\n },\n "last_name": "Weimann",\n "job": _\n "position": "Future Web Representative"\n },\n "first_name": "Brittany",\n "contacts": {\n _mobile__ "1-327-084-4643",\n "email": _\n "recusandae23@outlook.com"\n _\n }\n}</t>
+  </si>
+  <si>
+    <t>const customers =&gt; {\n "location": {\n "city"= "Crystal"\n },\n "last_name"= "Weimann",\n "job": {\n position: Future Web Representative\n },\n "first_name": "Brittany",\n "contacts"={}, {\n "mobile": "1-327-084-4643",\n "email": [\n "recusandae23@outlook.com"\n ]\n }\n]</t>
+  </si>
+  <si>
+    <t>const customers = {Æ "location": {Æ "city": "Crystal"Æ },Æ "last_name": "Weimann",Æ "job": {Æ "position": "Future Web Representative"Æ },Æ "first_name": "Brittany",Æ "contacts": {Æ "mobile": "1-327-084-4643",Æ "email": [Æ "recusandae23@outlook.com"Æ ]Æ }Æ}</t>
+  </si>
+  <si>
+    <t>Objects of Objects</t>
+  </si>
+  <si>
+    <t>const numbers = [\n 1234,\n [\'one\', \'two\', \'three\', \'four\'],\n \'five hundred\',\n [5, 0, 0]\n]</t>
+  </si>
+  <si>
+    <t>const numbers _ _\n 1234,\n _\'one\', \'two\', \'three\', \'four\'_,\n \'five hundred\',\n _5, 0, 0_\n_</t>
+  </si>
+  <si>
+    <t>const numbers = [\n 1234\n [\'one\' \'two\' \'three\' \'four\']\n \'five hundred\'\n [5 0 0]\n]</t>
+  </si>
+  <si>
+    <t>const numbers = [Æ 1234,Æ [\'one\', \'two\', \'three\', \'four\'],Æ \'five hundred\',Æ [5, 0, 0]Æ]</t>
+  </si>
+  <si>
+    <t>Arrays of Arrays</t>
+  </si>
+  <si>
+    <t>{\n "customers": [\n {\n "id": 1,\n "name": "Alice",\n "email": "alice@gmail.com"\n },\n {\n "id": 2,\n "name": "Bill",\n "email": "bill@gmail.com"\n }\n ],\n "balances": [\n {\n "id": 1,\n "customerId": 1,\n "accountBalance": 785.43\n },\n {\n "id": 2,\n "customerId": 2,\n "accountBalance": 23.81\n }\n ]\n}</t>
+  </si>
+  <si>
+    <t>{\n "customers": [\n {\n "__": 1,\n "name"_ "Alice",\n "_____": "alice@gmail.com"\n _,\n {\n "id": 2,\n "____": "Bill",\n "email": "bill@gmail.com"\n }\n ],\n "balances": _\n {\n "__": 1,\n "__________": 1,\n "accountBalance": 785.43\n _,\n {\n "id": 2,\n "customerId": _,\n "_______Balance": 23.81\n }\n ]\n}</t>
+  </si>
+  <si>
+    <t>[\n customers: {\n [\n id: 1,\n name: "Alice",\n email: "alice@gmail.com"\n ],\n {\n id: 2,\n name: "Bill",\n email: "bill@gmail.com"\n }\n ],\n balances: [\n {\n id: 1,\n customerId: 1,\n accountBalance: 785.43\n },\n {\n id: 2,\n customerId: 2,\n accountBalance: 23.81\n }\n }\n]</t>
+  </si>
+  <si>
+    <t>{Æ "customers": [Æ {Æ "id": 1,Æ "name": "Alice",Æ "email": "alice@gmail.com"Æ },Æ {Æ "id": 2,Æ "name": "Bill",Æ "email": "bill@gmail.com"Æ }Æ ],Æ "balances": [Æ {Æ "id": 1,Æ "customerId": 1,Æ "accountBalance": 785.43Æ },Æ {Æ "id": 2,Æ "customerId": 2,Æ "accountBalance": 23.81Æ }Æ ]Æ}</t>
+  </si>
+  <si>
+    <t>JSON</t>
+  </si>
+  <si>
+    <t>JSON Database</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Load from Session Storage</t>
+  </si>
+  <si>
+    <t>Load from Local Storage</t>
+  </si>
+  <si>
+    <t>const dbLoad = () =&gt; {\n const myData = sessionStorage.getItem(\'MyKey\')\n return JSON.parse(myData)\n}</t>
+  </si>
+  <si>
+    <t>_____ dbLoad = _____ {\n const myData = sessionStorage._______(\'MyKey\')\n return ____.parse(myData)\n}</t>
+  </si>
+  <si>
+    <t>const dbLoad = (function) : {\n const myData = sessionStorage.fetch(\'MyKey\')\n return JSON.sparse(myData)\n}</t>
+  </si>
+  <si>
+    <t>const dbLoad = () =&gt; {Æ const myData = sessionStorage.getItem(\'MyKey\')Æ return JSON.parse(myData)Æ}</t>
+  </si>
+  <si>
+    <t>const dbLoad = () =&gt; {\n const myData = localStorage.getItem(\'MyKey\')\n return JSON.parse(myData)\n}</t>
+  </si>
+  <si>
+    <t>_____ dbLoad = _____ {\n const myData = localStorage._______(\'MyKey\')\n return ____.parse(myData)\n}</t>
+  </si>
+  <si>
+    <t>const dbLoad = (function) : {\n const myData = localStorage.fetch(\'MyKey\')\n return JSON.sparse(myData)\n}</t>
+  </si>
+  <si>
+    <t>const dbLoad = () =&gt; {Æ const myData = localStorage.getItem(\'MyKey\')Æ return JSON.parse(myData)Æ}</t>
+  </si>
+  <si>
+    <t>const dbSave = (database) =&gt; {\n sessionStorage.setItem(\'MyKey\', JSON.stringify(database))\n}</t>
+  </si>
+  <si>
+    <t>const dbSave = (database) =&gt; {\n sessionStorage._____(\'MyKey\', JSON._________(database))\n}</t>
+  </si>
+  <si>
+    <t>const dbSave = {database} =&gt; {\n sessionStorage.setItem(\'MyKey\', JQUERY.spaghettify(database))\n}</t>
+  </si>
+  <si>
+    <t>const dbSave = (database) =&gt; {Æ sessionStorage.setItem(\'MyKey\', JSON.stringify(database))Æ}</t>
+  </si>
+  <si>
+    <t>Save to Session Storage</t>
+  </si>
+  <si>
+    <t>const dbSave = (database) =&gt; {\n localStorage.setItem(\'MyKey\', JSON.stringify(database))\n}</t>
+  </si>
+  <si>
+    <t>const dbSave = (database) =&gt; {\n localStorage._____(\'MyKey\', JSON._________(database))\n}</t>
+  </si>
+  <si>
+    <t>const dbSave = {database} =&gt; {\n localStorage.setItem(\'MyKey\', JQUERY.spaghettify(database))\n}</t>
+  </si>
+  <si>
+    <t>const dbSave = (database) =&gt; {Æ localStorage.setItem(\'MyKey\', JSON.stringify(database))Æ}</t>
+  </si>
+  <si>
+    <t>Save to Local Storage</t>
+  </si>
+  <si>
+    <t>document.querySelector(\'#news\').addEventListener(\'click\', function () {\n toggleClass(document.querySelector(\'#newsAlert\'), \'disabled\', \'enabled\')\n})</t>
+  </si>
+  <si>
+    <t>document.query________(\'#news\').___EventListener(\'click\', ________ () {\n toggleClass(document.querySelector(\'#newsAlert\'), \'disabled\', \'enabled\')\n})</t>
+  </si>
+  <si>
+    <t>document.selectSection(\'#news\').addSlistener(\'click\', =&gt; () {\n toggleClass(document.find(\'#newsAlert\'), \'disabled\', \'enabled\')\n})</t>
+  </si>
+  <si>
+    <t>document.querySelector(\'#news\').addEventListener(\'click\', function () {Æ toggleClass(document.querySelector(\'#newsAlert\'), \'disabled\', \'enabled\')Æ})</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Event Listeners in JavaScript</t>
+  </si>
+  <si>
+    <t>$(\'#form-button\').click(function() {\n console.log($(\'#input-name\').val())\n})</t>
+  </si>
+  <si>
+    <t>$(\'#form-button\')._____(function__ {\n console.log($(\'#input-name\').val___\n})</t>
+  </si>
+  <si>
+    <t>$(\'#form-button\').slick(unction() [\n console.log(!(\'#input-name\').val())\n])</t>
+  </si>
+  <si>
+    <t>$(\'#form-button\').click(function() {Æ console.log($(\'#input-name\').val())Æ})</t>
+  </si>
+  <si>
+    <t>jQuery</t>
+  </si>
+  <si>
+    <t>Event Listeners in jQuery</t>
+  </si>
+  <si>
+    <t>$(\'.main-article\').mouseover(function(){\n console.log(\'The mouse is moving!\')\n})</t>
+  </si>
+  <si>
+    <t>$(\'.main-article\')._____over(________(){\n console.log(\'The mouse is moving!\')\n})</t>
+  </si>
+  <si>
+    <t>$(\'.main-article\').onMouseOver(=&gt;(){\n console.vlog(\'The mouse is being still!\')\n})</t>
+  </si>
+  <si>
+    <t>$(\'.main-article\').mouseover(function(){Æ console.log(\'The mouse is moving!\')Æ})</t>
+  </si>
+  <si>
+    <t>Animations</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>$(\'#button\').click(function(){\n $(\'#myImage\').animate(\n {\n opacity: 0.5,\n width: \'100%\'\n }\n )\n })</t>
+  </si>
+  <si>
+    <t>$(\'#button\').click(function(){\n ____myImage\')._______(\n {\n opacity: 0.5,\n width: \'100%\'\n _\n )\n })</t>
+  </si>
+  <si>
+    <t>$(\'#button\').activate(animate(){\n $(\'#myImage\').moveLeft(\n {\n opacity: 0.5,\n width: \'100%\'\n }\n )\n })</t>
+  </si>
+  <si>
+    <t>$(\'#button\').click(function(){Æ $(\'#myImage\').animate(Æ {Æ opacity: 0.5,Æ width: \'100%\'Æ }Æ )Æ })</t>
+  </si>
+  <si>
+    <t>Fade Effects</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">if (i % 5 === 0 </t>
     </r>
@@ -811,7 +1248,7 @@
         <rFont val="Fira Code"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> i % 7 === 0) {\n console.log('ChickenMonkey')\n}</t>
+      <t xml:space="preserve"> i % 7 === 0) {\n console.log(\'ChickenMonkey\')\n}</t>
     </r>
   </si>
   <si>
@@ -834,7 +1271,7 @@
         <rFont val="Fira Code"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> i _ 7 === 0) {\n console.log('ChickenMonkey')\n}</t>
+      <t xml:space="preserve"> i _ 7 === 0) {\n console.log(\'ChickenMonkey\')\n}</t>
     </r>
   </si>
   <si>
@@ -857,7 +1294,7 @@
         <rFont val="Fira Code"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> i # 7 = 0) (\n console.blog('ChickenMonkey')\n)</t>
+      <t xml:space="preserve"> i # 7 = 0) (\n console.blog(\'ChickenMonkey\')\n)</t>
     </r>
   </si>
   <si>
@@ -880,18 +1317,18 @@
         <rFont val="Fira Code"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> i % 7 === 0) {Æ console.log('ChickenMonkey')Æ}</t>
-    </r>
-  </si>
-  <si>
-    <t>If Condition</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">for (let i = 0; i </t>
+      <t xml:space="preserve"> i % 7 === 0) {Æ console.log(\'ChickenMonkey\')Æ}</t>
+    </r>
+  </si>
+  <si>
+    <t>const cookies = [\'chocolate chip\', \'peanut butter\']\ncookies.forEach(cookie =&gt; {\n console.log(`That's a tasty ${cookie} cookie!`)\n})</t>
+  </si>
+  <si>
+    <t>const cookies = _\'chocolate chip\'_ \'peanut butter\'_\ncookies.forEach(cookie __ {\n _______.log(_That's a tasty ${cookie} cookie!_)\n})</t>
+  </si>
+  <si>
+    <r>
+      <t>const cookies = {\'chocolate chip\'</t>
     </r>
     <r>
       <rPr>
@@ -900,87 +1337,6 @@
         <rFont val="Fira Code"/>
         <family val="3"/>
       </rPr>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBB1C9"/>
-        <rFont val="Fira Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>= 100; i++) {\n string += a\n}</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">for (___ i = 0; i </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCF433E"/>
-        <rFont val="Fira Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBB1C9"/>
-        <rFont val="Fira Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>= 100; i__) {\n string += a\n}</t>
-    </r>
-  </si>
-  <si>
-    <t>while (vet i = 0; i = 100; i--) {\n string += a\n}</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">for (let i = 0; i </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCF433E"/>
-        <rFont val="Fira Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>&lt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFBBB1C9"/>
-        <rFont val="Fira Code"/>
-        <family val="3"/>
-      </rPr>
-      <t>= 100; i++) {Æ string += aÆ}</t>
-    </r>
-  </si>
-  <si>
-    <t>For Loop</t>
-  </si>
-  <si>
-    <t>const cookies = ['chocolate chip', 'peanut butter']\ncookies.forEach(cookie =&gt; {\n console.log(`That's a tasty ${cookie} cookie!`)\n})</t>
-  </si>
-  <si>
-    <t>const cookies = _'chocolate chip'_ 'peanut butter'_\ncookies.forEach(cookie __ {\n _______.log(_That's a tasty ${cookie} cookie!_)\n})</t>
-  </si>
-  <si>
-    <r>
-      <t>const cookies = {'chocolate chip'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFCF433E"/>
-        <rFont val="Fira Code"/>
-        <family val="3"/>
-      </rPr>
       <t>&amp;</t>
     </r>
     <r>
@@ -990,14 +1346,619 @@
         <rFont val="Fira Code"/>
         <family val="3"/>
       </rPr>
-      <t xml:space="preserve"> 'peanut butter'}\ncookies.for (cookie =&gt; {\n console.log("That's a tasty {cookie} cookie!")\n})</t>
-    </r>
-  </si>
-  <si>
-    <t>const cookies = ['chocolate chip', 'peanut butter']Æcookies.forEach(cookie =&gt; {Æ console.log(`That's a tasty ${cookie} cookie!`)Æ})</t>
-  </si>
-  <si>
-    <t>ForEach Loop</t>
+      <t xml:space="preserve"> \'peanut butter\'}\ncookies.for (cookie =&gt; {\n console.log("That's a tasty {cookie} cookie!")\n})</t>
+    </r>
+  </si>
+  <si>
+    <t>const cookies = [\'chocolate chip\', \'peanut butter\']Æcookies.forEach(cookie =&gt; {Æ console.log(`That's a tasty ${cookie} cookie!`)Æ})</t>
+  </si>
+  <si>
+    <t>$(\'#button\').click(function(){\n $(\'#myImage\').fadeOut(1000)\n $(\'#myImage\').fadeIn(\'slow\')\n})</t>
+  </si>
+  <si>
+    <t>$(\'#button\')._____(function(){\n ____myImage\').fadeOut(1000)\n $(\'#myImage\').fade__(\'slow\')\n})</t>
+  </si>
+  <si>
+    <t>!(\'#button\').flick(handler(){\n !(\'#myImage\').fadeOut(1000)\n !(\'#myImage\').shimmy(\'slow\')\n})</t>
+  </si>
+  <si>
+    <t>$(\'#button\').click(function(){Æ $(\'#myImage\').fadeOut(1000)Æ $(\'#myImage\').fadeIn(\'slow\')Æ})</t>
+  </si>
+  <si>
+    <t>$(\'#loadSongs\').click(function(){\n $.ajax({ url: \'data.json\', method: "GET"})\n .then(response =&gt; {\n //do something\n })\n})</t>
+  </si>
+  <si>
+    <t>____loadSongs\').click(function(){\n $.____({ url: \'data.json\', method: "___"})\n .then(response =&gt; {\n //do something\n })\n})</t>
+  </si>
+  <si>
+    <t>const loader = () =&gt; {$(\'#loadSongs\').click(function(){\n $.ajax({ url: \'data.json\', method: "FETCH"})\n .then(response =&gt; {\n //do something\n })\n})</t>
+  </si>
+  <si>
+    <t>$(\'#loadSongs\').click(function(){Æ $.ajax({ url: \'data.json\', method: "GET"})Æ .then(response =&gt; {Æ //do somethingÆ })Æ})</t>
+  </si>
+  <si>
+    <t>AJAX Get</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>json-server -p 5001 -w db.json</t>
+  </si>
+  <si>
+    <t>json-______ -p 5001 -w db.____</t>
+  </si>
+  <si>
+    <t>$(jquery)json-server --fetch all 5001 -w db.json</t>
+  </si>
+  <si>
+    <t>Starting JSON-Server</t>
+  </si>
+  <si>
+    <t>let promises = []\npromises.push(\n //something from the API\n)\nPromise.all(promises).then(result =&gt; {\n //do something else\n})</t>
+  </si>
+  <si>
+    <t>let promises = __\npromises.push(\n //something from the API\n)\nPromise.___(promises).____(result =&gt; {\n //do something else\n})</t>
+  </si>
+  <si>
+    <t>let promises = {}\npromises.push(\n //something from the API\n)\nPromise.swear(promises).then(result = {\n //do something else\n})</t>
+  </si>
+  <si>
+    <t>let promises = []Æpromises.push(Æ //something from the APIÆ)ÆPromise.all(promises).then(result =&gt; {Æ //do something elseÆ})</t>
+  </si>
+  <si>
+    <t>Promise.all</t>
+  </si>
+  <si>
+    <t>import React, { Component } from "react"</t>
+  </si>
+  <si>
+    <t>import React, { _________ } from "_____"</t>
+  </si>
+  <si>
+    <t>return React, { Module } from "react"</t>
+  </si>
+  <si>
+    <t>React Import Statement</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>export default class MyClass extends Component {}</t>
+  </si>
+  <si>
+    <t>export _______ class MyClass extends _________ {}</t>
+  </si>
+  <si>
+    <t>import class MyClass extends React {}</t>
+  </si>
+  <si>
+    <t>React Export Statement</t>
+  </si>
+  <si>
+    <r>
+      <t>render() {\n return (\n &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Title&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n )\n}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>render() {\n ______ (\n &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Title&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n )\n}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>return() {\n const element = (\n &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Title&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Hey!&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;\n )\n}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>render() {Æ return (Æ &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Æ &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Title&lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Æ &lt;/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>div</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>&gt;Æ )Æ}</t>
+    </r>
+  </si>
+  <si>
+    <t>React Render Function</t>
+  </si>
+  <si>
+    <r>
+      <t>this.props.myArray.map(element =&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>MyComponent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7C617C"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>key</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE5C71B"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{element.id}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> /&gt;)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>this._____.myArray.map(element =&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>MyComponent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> ___=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE5C71B"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{element.id}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> __)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>props.myArray.filter(element (function) =&gt; &lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFC814A"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>MyComponent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7C617C"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFE5C71B"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t>{element.id}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFBBB1C9"/>
+        <rFont val="Fira Code"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> /&gt;)</t>
+    </r>
+  </si>
+  <si>
+    <t>Props in React</t>
+  </si>
+  <si>
+    <t>state = {\n userName: \'\',\n userId: \'\'\n}</t>
+  </si>
+  <si>
+    <t>state = _\n userName: \'\',\n userId_ \'\'\n}</t>
+  </si>
+  <si>
+    <t>stuff = [\n userName: (\'\'),\n userId: \'\'\n]</t>
+  </si>
+  <si>
+    <t>React State</t>
+  </si>
+  <si>
+    <t>state = {Æ userName: \'\',Æ userId: \'\'Æ}</t>
   </si>
 </sst>
 </file>
@@ -1397,11 +2358,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F59CDE06-17D5-49D9-8E96-716BBD57AB89}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,7 +2428,7 @@
         <v>10</v>
       </c>
       <c r="I2" s="4" t="str">
-        <f t="shared" ref="I2:I20" si="0">_xlfn.CONCAT("create_CodeBlock('",B2,"', '",C2,"', ",D2,", '",E2,"', '",F2,"', '",G2,"', '",H2,"')")</f>
+        <f t="shared" ref="I2:I50" si="0">_xlfn.CONCAT("create_CodeBlock('",B2,"', '",C2,"', ",D2,", '",E2,"', '",F2,"', '",G2,"', '",H2,"')")</f>
         <v>create_CodeBlock('JavaScript', 'Declaring Variables', 0, 'const a = 1\nconst b = \'string\'\nconst c = a + b', 'const _ = 1\nconst b = _string_\n_____ c = a _ b', 'var a = 1\nconst b = string\nconst c = a &amp; b', 'const a = 1Æconst b = \'string\'Æconst c = a + b')</v>
       </c>
     </row>
@@ -1881,26 +2842,26 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>89</v>
+        <v>207</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>90</v>
+        <v>208</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>91</v>
+        <v>209</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>92</v>
+        <v>210</v>
       </c>
       <c r="I18" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>create_CodeBlock('JavaScript', 'If Condition', 3, 'if (i % 5 === 0 &amp;&amp; i % 7 === 0) {\n console.log('ChickenMonkey')\n}', 'if (i % 5 ___ 0 &amp;&amp; i _ 7 === 0) {\n console.log('ChickenMonkey')\n}', 'if (i # 5 = 0 &amp;&amp; i # 7 = 0) (\n console.blog('ChickenMonkey')\n)', 'if (i % 5 === 0 &amp;&amp; i % 7 === 0) {Æ console.log('ChickenMonkey')Æ}')</v>
+        <v>create_CodeBlock('JavaScript', 'If Condition', 3, 'if (i % 5 === 0 &amp;&amp; i % 7 === 0) {\n console.log(\'ChickenMonkey\')\n}', 'if (i % 5 ___ 0 &amp;&amp; i _ 7 === 0) {\n console.log(\'ChickenMonkey\')\n}', 'if (i # 5 = 0 &amp;&amp; i # 7 = 0) (\n console.blog(\'ChickenMonkey\')\n)', 'if (i % 5 === 0 &amp;&amp; i % 7 === 0) {Æ console.log(\'ChickenMonkey\')Æ}')</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
@@ -1908,22 +2869,22 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="I19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1935,29 +2896,840 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="I20" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'ForEach Loop', 3, 'const cookies = [\'chocolate chip\', \'peanut butter\']\ncookies.forEach(cookie =&gt; {\n console.log(`That's a tasty ${cookie} cookie!`)\n})', 'const cookies = _\'chocolate chip\'_ \'peanut butter\'_\ncookies.forEach(cookie __ {\n _______.log(_That's a tasty ${cookie} cookie!_)\n})', 'const cookies = {\'chocolate chip\'&amp; \'peanut butter\'}\ncookies.for (cookie =&gt; {\n console.log("That's a tasty {cookie} cookie!")\n})', 'const cookies = [\'chocolate chip\', \'peanut butter\']Æcookies.forEach(cookie =&gt; {Æ console.log(`That's a tasty ${cookie} cookie!`)Æ})')</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="I21" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Interpolation', 3, 'const conjunction = (firstWord, secondWord) =&gt; {\n return `${firstWord} ${secondWord}`\n}\nconsole.log(conjunction(\'Master\', \'Card\'))', '_____ conjunction = (firstWord, secondWord) __ {\n return ___firstWord} ${secondWord}`\n}\nconsole.___(___________(\'Master\', \'Card\'))', 'const conjunction = (\'firstWord\', \'secondWord\') : {\n return `\'firstWord\' 'secondWord'`\n}\nxbox.console(conjunction(\'Master\', \'Card\'))', 'const conjunction = (firstWord, secondWord) =&gt; {Æ return `${firstWord} ${secondWord}`Æ}Æconsole.log(conjunction(\'Master\', \'Card\'))')</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I20" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>create_CodeBlock('JavaScript', 'ForEach Loop', 3, 'const cookies = ['chocolate chip', 'peanut butter']\ncookies.forEach(cookie =&gt; {\n console.log(`That's a tasty ${cookie} cookie!`)\n})', 'const cookies = _'chocolate chip'_ 'peanut butter'_\ncookies.forEach(cookie __ {\n _______.log(_That's a tasty ${cookie} cookie!_)\n})', 'const cookies = {'chocolate chip'&amp; 'peanut butter'}\ncookies.for (cookie =&gt; {\n console.log("That's a tasty {cookie} cookie!")\n})', 'const cookies = ['chocolate chip', 'peanut butter']Æcookies.forEach(cookie =&gt; {Æ console.log(`That's a tasty ${cookie} cookie!`)Æ})')</v>
+      <c r="H22" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I22" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('CSS', 'Nested CSS', 3, 'nav ul li {\n display: inline;\n padding: 2em;\n}', 'nav ul li _\n display: inline;\n padding: 2__;\n}', 'nav ul li (\n show: online;\n space-around: 2em;\n)', 'nav ul li {Æ display: inline;Æ padding: 2em;Æ}')</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Creating Objects', 4, 'const steve = {\n name: \'Steve Brownlee\',\n job: \'Instructor\'\n}', '_____ steve _ {\n name_ _Steve Brownlee_,\n ___: \'Instructor\'\n_', 'create steve = [\n name: \'Steve Brownlee\',\n job: \'Rock Star\'\n]', 'const steve = {Æ name: \'Steve Brownlee\',Æ job: \'Instructor\'Æ}')</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="I24" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Object.create', 4, 'const person = Object.create({}, {\n name: {\n value: \'Kimmy Bird\',\n enumerable: true\n },\n job: {\n value: \'Instructor\',\n enumerable: true\n }\n})', 'const person = ______.______(__, {\n name: {\n _____: \'Kimmy Bird\',\n enumerable: ____\n },\n job: {\n value: _Instructor_,\n __________: true\n }\n})', 'create person = Object.spawn({\n name: {\n value: \'Kimmy Bird\',\n enumberable: true\n },\n job: {\n value: \'Code Wizard\',\n enumerable: false\n }\n})', 'const person = Object.create({}, {Æ name: {Æ value: \'Kimmy Bird\',Æ enumerable: trueÆ },Æ job: {Æ value: \'Instructor\',Æ enumerable: trueÆ }Æ})')</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="I25" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Array Maps', 4, 'const capPlanets = planets.map(planet =&gt; {\n return planet.charAt(0).toUpperCase() + planet.slice(1)\n})', 'const capPlanets = planets.___(planet __ {\n ______ planet.charAt(0).toUpperCase() + ______.slice(1)\n})', 'const capPlanets = planets.map((function) planet =&gt; {\n return planet.characterAt(0).toUpper() + planet.lice(1)\n})', 'const capPlanets = planets.map(planet =&gt; {Æ return planet.charAt(0).toUpperCase() + planet.slice(1)Æ})')</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I26" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Array Filters', 4, 'const filteredPlanets = planets.filter(planet =&gt; {\n const containsE = planet.includes(\'e\')\n return containsE\n})', 'const filteredPlanets = planets.______(planet =&gt; {\n _____ containsE = planet.includes(\'_\')\n return _________\n})', 'const filteredPlanets = planets.addFilter(planet (function) {\n if containsE = planet.hasCharmander(\'e\')\n provide containsE\n})', 'const filteredPlanets = planets.filter(planet =&gt; {Æ const containsE = planet.includes(\'e\')Æ return containsEÆ})')</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="I27" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Array Reduce', 4, 'const words = [\'an\', \'early\', \'bird\']\nconst sentence = words.reduce(\n   (partial, next) =&gt; partial + \' \' + next\n)', 'const words = _\'an\', \'early\', \'bird\'_\nconst sentence = _____.reduce(\n   (partial, next) __ partial + \' \' + ____\n)', 'const words = [an, early, bird]\nconst sentence = words.induce(\n   (partial &amp; next) = partial + \' \' + next\n)', 'const words = [\'an\', \'early\', \'bird\']Æconst sentence = words.reduce(Æ (partial, next) =&gt; partial + \' \' + nextÆ)')</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="I28" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('CSS', 'Nested CSS', 5, '.top li {\n list-style: none;\n display: inline;\n}', '.top li {\n list-_____: none;\n _______: inline;\n}', '.top li {\n list-style: noBullet;\n display: true;\n}', '.top li {Æ list-style: none;Æ display: inline;Æ}')</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="I29" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('CSS', 'CSS Pseudo Selectors', 5, '.n-child section:nth-of-type(even){\n border: 1px solid green;\n}', '.n-child section:___-of-type(even){\n border: ___ solid green;\n}', '.n-child section:4th-oft-hype(steven){\n border: solid green 1px;\n}', '.n-child section:nth-of-type(even){Æ border: 1px solid green;Æ}')</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="I30" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('CSS', 'CSS Pseudo Selectors', 5, '.top li:not(:last-child)::after {\n content: \',\';\n}', '.top li:___(:____-child)__after {\n content: \',\';\n}', '.top li:not(:last-parent)::while {\n content: \';\n}', '.top li:not(:last-child)::after {Æ content: \',\';Æ}')</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I31" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Objects of Objects', 5, 'const customers = {\n "location": {\n "city": "Crystal"\n },\n "last_name": "Weimann",\n "job": {\n "position": "Future Web Representative"\n },\n "first_name": "Brittany",\n "contacts": {\n "mobile": "1-327-084-4643",\n "email": [\n "recusandae23@outlook.com"\n ]\n }\n}', '_____ customers = {\n "location": {\n _city_: "Crystal"\n },\n "last_name": "Weimann",\n "job": _\n "position": "Future Web Representative"\n },\n "first_name": "Brittany",\n "contacts": {\n _mobile__ "1-327-084-4643",\n "email": _\n "recusandae23@outlook.com"\n _\n }\n}', 'const customers =&gt; {\n "location": {\n "city"= "Crystal"\n },\n "last_name"= "Weimann",\n "job": {\n position: Future Web Representative\n },\n "first_name": "Brittany",\n "contacts"={}, {\n "mobile": "1-327-084-4643",\n "email": [\n "recusandae23@outlook.com"\n ]\n }\n]', 'const customers = {Æ "location": {Æ "city": "Crystal"Æ },Æ "last_name": "Weimann",Æ "job": {Æ "position": "Future Web Representative"Æ },Æ "first_name": "Brittany",Æ "contacts": {Æ "mobile": "1-327-084-4643",Æ "email": [Æ "recusandae23@outlook.com"Æ ]Æ }Æ}')</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="I32" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Arrays of Arrays', 5, 'const numbers = [\n 1234,\n [\'one\', \'two\', \'three\', \'four\'],\n \'five hundred\',\n [5, 0, 0]\n]', 'const numbers _ _\n 1234,\n _\'one\', \'two\', \'three\', \'four\'_,\n \'five hundred\',\n _5, 0, 0_\n_', 'const numbers = [\n 1234\n [\'one\' \'two\' \'three\' \'four\']\n \'five hundred\'\n [5 0 0]\n]', 'const numbers = [Æ 1234,Æ [\'one\', \'two\', \'three\', \'four\'],Æ \'five hundred\',Æ [5, 0, 0]Æ]')</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="I33" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JSON', 'JSON Database', 6, '{\n "customers": [\n {\n "id": 1,\n "name": "Alice",\n "email": "alice@gmail.com"\n },\n {\n "id": 2,\n "name": "Bill",\n "email": "bill@gmail.com"\n }\n ],\n "balances": [\n {\n "id": 1,\n "customerId": 1,\n "accountBalance": 785.43\n },\n {\n "id": 2,\n "customerId": 2,\n "accountBalance": 23.81\n }\n ]\n}', '{\n "customers": [\n {\n "__": 1,\n "name"_ "Alice",\n "_____": "alice@gmail.com"\n _,\n {\n "id": 2,\n "____": "Bill",\n "email": "bill@gmail.com"\n }\n ],\n "balances": _\n {\n "__": 1,\n "__________": 1,\n "accountBalance": 785.43\n _,\n {\n "id": 2,\n "customerId": _,\n "_______Balance": 23.81\n }\n ]\n}', '[\n customers: {\n [\n id: 1,\n name: "Alice",\n email: "alice@gmail.com"\n ],\n {\n id: 2,\n name: "Bill",\n email: "bill@gmail.com"\n }\n ],\n balances: [\n {\n id: 1,\n customerId: 1,\n accountBalance: 785.43\n },\n {\n id: 2,\n customerId: 2,\n accountBalance: 23.81\n }\n }\n]', '{Æ "customers": [Æ {Æ "id": 1,Æ "name": "Alice",Æ "email": "alice@gmail.com"Æ },Æ {Æ "id": 2,Æ "name": "Bill",Æ "email": "bill@gmail.com"Æ }Æ ],Æ "balances": [Æ {Æ "id": 1,Æ "customerId": 1,Æ "accountBalance": 785.43Æ },Æ {Æ "id": 2,Æ "customerId": 2,Æ "accountBalance": 23.81Æ }Æ ]Æ}')</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I34" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Load from Session Storage', 6, 'const dbLoad = () =&gt; {\n const myData = sessionStorage.getItem(\'MyKey\')\n return JSON.parse(myData)\n}', '_____ dbLoad = _____ {\n const myData = sessionStorage._______(\'MyKey\')\n return ____.parse(myData)\n}', 'const dbLoad = (function) : {\n const myData = sessionStorage.fetch(\'MyKey\')\n return JSON.sparse(myData)\n}', 'const dbLoad = () =&gt; {Æ const myData = sessionStorage.getItem(\'MyKey\')Æ return JSON.parse(myData)Æ}')</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="I35" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Load from Local Storage', 6, 'const dbLoad = () =&gt; {\n const myData = localStorage.getItem(\'MyKey\')\n return JSON.parse(myData)\n}', '_____ dbLoad = _____ {\n const myData = localStorage._______(\'MyKey\')\n return ____.parse(myData)\n}', 'const dbLoad = (function) : {\n const myData = localStorage.fetch(\'MyKey\')\n return JSON.sparse(myData)\n}', 'const dbLoad = () =&gt; {Æ const myData = localStorage.getItem(\'MyKey\')Æ return JSON.parse(myData)Æ}')</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="I36" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Save to Session Storage', 6, 'const dbSave = (database) =&gt; {\n sessionStorage.setItem(\'MyKey\', JSON.stringify(database))\n}', 'const dbSave = (database) =&gt; {\n sessionStorage._____(\'MyKey\', JSON._________(database))\n}', 'const dbSave = {database} =&gt; {\n sessionStorage.setItem(\'MyKey\', JQUERY.spaghettify(database))\n}', 'const dbSave = (database) =&gt; {Æ sessionStorage.setItem(\'MyKey\', JSON.stringify(database))Æ}')</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I37" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Save to Local Storage', 6, 'const dbSave = (database) =&gt; {\n localStorage.setItem(\'MyKey\', JSON.stringify(database))\n}', 'const dbSave = (database) =&gt; {\n localStorage._____(\'MyKey\', JSON._________(database))\n}', 'const dbSave = {database} =&gt; {\n localStorage.setItem(\'MyKey\', JQUERY.spaghettify(database))\n}', 'const dbSave = (database) =&gt; {Æ localStorage.setItem(\'MyKey\', JSON.stringify(database))Æ}')</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="I38" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Event Listeners in JavaScript', 7, 'document.querySelector(\'#news\').addEventListener(\'click\', function () {\n toggleClass(document.querySelector(\'#newsAlert\'), \'disabled\', \'enabled\')\n})', 'document.query________(\'#news\').___EventListener(\'click\', ________ () {\n toggleClass(document.querySelector(\'#newsAlert\'), \'disabled\', \'enabled\')\n})', 'document.selectSection(\'#news\').addSlistener(\'click\', =&gt; () {\n toggleClass(document.find(\'#newsAlert\'), \'disabled\', \'enabled\')\n})', 'document.querySelector(\'#news\').addEventListener(\'click\', function () {Æ toggleClass(document.querySelector(\'#newsAlert\'), \'disabled\', \'enabled\')Æ})')</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="I39" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('jQuery', 'Event Listeners in jQuery', 7, '$(\'#form-button\').click(function() {\n console.log($(\'#input-name\').val())\n})', '$(\'#form-button\')._____(function__ {\n console.log($(\'#input-name\').val___\n})', '$(\'#form-button\').slick(unction() [\n console.log(!(\'#input-name\').val())\n])', '$(\'#form-button\').click(function() {Æ console.log($(\'#input-name\').val())Æ})')</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="I40" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('jQuery', 'Event Listeners in jQuery', 7, '$(\'.main-article\').mouseover(function(){\n console.log(\'The mouse is moving!\')\n})', '$(\'.main-article\')._____over(________(){\n console.log(\'The mouse is moving!\')\n})', '$(\'.main-article\').onMouseOver(=&gt;(){\n console.vlog(\'The mouse is being still!\')\n})', '$(\'.main-article\').mouseover(function(){Æ console.log(\'The mouse is moving!\')Æ})')</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="I41" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('jQuery', 'Fade Effects', 8, '$(\'#button\').click(function(){\n $(\'#myImage\').fadeOut(1000)\n $(\'#myImage\').fadeIn(\'slow\')\n})', '$(\'#button\')._____(function(){\n ____myImage\').fadeOut(1000)\n $(\'#myImage\').fade__(\'slow\')\n})', '!(\'#button\').flick(handler(){\n !(\'#myImage\').fadeOut(1000)\n !(\'#myImage\').shimmy(\'slow\')\n})', '$(\'#button\').click(function(){Æ $(\'#myImage\').fadeOut(1000)Æ $(\'#myImage\').fadeIn(\'slow\')Æ})')</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="I42" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('jQuery', 'Animations', 8, '$(\'#button\').click(function(){\n $(\'#myImage\').animate(\n {\n opacity: 0.5,\n width: \'100%\'\n }\n )\n })', '$(\'#button\').click(function(){\n ____myImage\')._______(\n {\n opacity: 0.5,\n width: \'100%\'\n _\n )\n })', '$(\'#button\').activate(animate(){\n $(\'#myImage\').moveLeft(\n {\n opacity: 0.5,\n width: \'100%\'\n }\n )\n })', '$(\'#button\').click(function(){Æ $(\'#myImage\').animate(Æ {Æ opacity: 0.5,Æ width: \'100%\'Æ }Æ )Æ })')</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I43" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('jQuery', 'AJAX Get', 9, '$(\'#loadSongs\').click(function(){\n $.ajax({ url: \'data.json\', method: "GET"})\n .then(response =&gt; {\n //do something\n })\n})', '____loadSongs\').click(function(){\n $.____({ url: \'data.json\', method: "___"})\n .then(response =&gt; {\n //do something\n })\n})', 'const loader = () =&gt; {$(\'#loadSongs\').click(function(){\n $.ajax({ url: \'data.json\', method: "FETCH"})\n .then(response =&gt; {\n //do something\n })\n})', '$(\'#loadSongs\').click(function(){Æ $.ajax({ url: \'data.json\', method: "GET"})Æ .then(response =&gt; {Æ //do somethingÆ })Æ})')</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="I44" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('Command Line', 'Starting JSON-Server', 9, 'json-server -p 5001 -w db.json', 'json-______ -p 5001 -w db.____', '$(jquery)json-server --fetch all 5001 -w db.json', 'json-server -p 5001 -w db.json')</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="I45" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Promise.all', 9, 'let promises = []\npromises.push(\n //something from the API\n)\nPromise.all(promises).then(result =&gt; {\n //do something else\n})', 'let promises = __\npromises.push(\n //something from the API\n)\nPromise.___(promises).____(result =&gt; {\n //do something else\n})', 'let promises = {}\npromises.push(\n //something from the API\n)\nPromise.swear(promises).then(result = {\n //do something else\n})', 'let promises = []Æpromises.push(Æ //something from the APIÆ)ÆPromise.all(promises).then(result =&gt; {Æ //do something elseÆ})')</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="I46" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'React Import Statement', 10, 'import React, { Component } from "react"', 'import React, { _________ } from "_____"', 'return React, { Module } from "react"', 'import React, { Component } from "react"')</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="I47" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'React Export Statement', 10, 'export default class MyClass extends Component {}', 'export _______ class MyClass extends _________ {}', 'import class MyClass extends React {}', 'export default class MyClass extends Component {}')</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="I48" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'React Render Function', 10, 'render() {\n return (\n &lt;div&gt;\n &lt;h1&gt;Title&lt;/h1&gt;\n &lt;/div&gt;\n )\n}', 'render() {\n ______ (\n &lt;div&gt;\n &lt;h1&gt;Title&lt;/h1&gt;\n &lt;/div&gt;\n )\n}', 'return() {\n const element = (\n &lt;div&gt;\n &lt;h1&gt;Title&lt;/h1&gt;\n &lt;/div&gt;&lt;p&gt;Hey!&lt;/p&gt;\n )\n}', 'render() {Æ return (Æ &lt;div&gt;Æ &lt;h1&gt;Title&lt;/h1&gt;Æ &lt;/div&gt;Æ )Æ}')</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="I49" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'Props in React', 10, 'this.props.myArray.map(element =&gt; &lt;MyComponent key={element.id} /&gt;)', 'this._____.myArray.map(element =&gt; &lt;MyComponent ___={element.id} __)', 'props.myArray.filter(element (function) =&gt; &lt;MyComponent id={element.id} /&gt;)', 'this.props.myArray.map(element =&gt; &lt;MyComponent key={element.id} /&gt;)')</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="I50" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>create_CodeBlock('JavaScript', 'React State', 10, 'state = {\n userName: \'\',\n userId: \'\'\n}', 'state = _\n userName: \'\',\n userId_ \'\'\n}', 'stuff = [\n userName: (\'\'),\n userId: \'\'\n]', 'state = {Æ userName: \'\',Æ userId: \'\'Æ}')</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I50" xr:uid="{29CD1002-1A1A-4124-B2C8-B2C01BA50B5C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
code block minigame validation is fully operational.
</commit_message>
<xml_diff>
--- a/src/scripts/CodeBlocks/code blocks.xlsx
+++ b/src/scripts/CodeBlocks/code blocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin of the Lake\workspace\Repos\FrontEndCapstone\src\scripts\CodeBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7462C33F-4AFC-4F1C-9F3D-E2040D0673EE}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D00E843-CF1D-4804-9214-EBF04E4DBEB9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="9285" xr2:uid="{CB3B7D12-EE88-4088-ADA6-0AA53F93C8FE}"/>
   </bookViews>
@@ -651,18 +651,6 @@
     <t>CSS Button Styling</t>
   </si>
   <si>
-    <t>const myFunction = () =&gt; {\n const str1 = \'some text\'\n console.log\nstr1.length)\n}</t>
-  </si>
-  <si>
-    <t>const myFunction = __ __ {\n _____ str1 = \'some text\'\n console.___\nstr1.length)\n}</t>
-  </si>
-  <si>
-    <t>var myFunction = (is perfect) = {\n str1 = some text\n console.slog\nstr1.lenth)\n}</t>
-  </si>
-  <si>
-    <t>const myFunction = () =&gt; {Æ const str1 = \'some text\'Æ console.logÆstr1.length)Æ}</t>
-  </si>
-  <si>
     <t>Arrow Functions</t>
   </si>
   <si>
@@ -1959,6 +1947,18 @@
   </si>
   <si>
     <t>state = {Æ userName: \'\',Æ userId: \'\'Æ}</t>
+  </si>
+  <si>
+    <t>const myFunction = () =&gt; {\n const str1 = \'some text\'\n console.log(str1.length)\n}</t>
+  </si>
+  <si>
+    <t>const myFunction = __ __ {\n _____ str1 = \'some text\'\n console.___(str1.length)\n}</t>
+  </si>
+  <si>
+    <t>var myFunction = (is perfect) = {\n str1 = some text\n console.slog(str1.lenth)\n}</t>
+  </si>
+  <si>
+    <t>const myFunction = () =&gt; {Æ const str1 = \'some text\'Æ console.log(str1.length)Æ}</t>
   </si>
 </sst>
 </file>
@@ -2362,7 +2362,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2572,49 +2572,49 @@
         <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>41</v>
+        <v>253</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>254</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>43</v>
+        <v>255</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>44</v>
+        <v>256</v>
       </c>
       <c r="I8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>create_CodeBlock('JavaScript', 'Arrow Functions', 1, 'const myFunction = () =&gt; {\n const str1 = \'some text\'\n console.log\nstr1.length)\n}', 'const myFunction = __ __ {\n _____ str1 = \'some text\'\n console.___\nstr1.length)\n}', 'var myFunction = (is perfect) = {\n str1 = some text\n console.slog\nstr1.lenth)\n}', 'const myFunction = () =&gt; {Æ const str1 = \'some text\'Æ console.logÆstr1.length)Æ}')</v>
+        <v>create_CodeBlock('JavaScript', 'Arrow Functions', 1, 'const myFunction = () =&gt; {\n const str1 = \'some text\'\n console.log(str1.length)\n}', 'const myFunction = __ __ {\n _____ str1 = \'some text\'\n console.___(str1.length)\n}', 'var myFunction = (is perfect) = {\n str1 = some text\n console.slog(str1.lenth)\n}', 'const myFunction = () =&gt; {Æ const str1 = \'some text\'Æ console.log(str1.length)Æ}')</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="I9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2623,25 +2623,25 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>54</v>
-      </c>
       <c r="H10" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2650,25 +2650,25 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2677,25 +2677,25 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I12" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2704,25 +2704,25 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="2" t="s">
+      <c r="H13" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="I13" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2734,22 +2734,22 @@
         <v>11</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I14" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2761,22 +2761,22 @@
         <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I15" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2785,25 +2785,25 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I16" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2812,25 +2812,25 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I17" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2842,22 +2842,22 @@
         <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I18" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2869,22 +2869,22 @@
         <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="I19" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2896,22 +2896,22 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I20" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2923,22 +2923,22 @@
         <v>11</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="I21" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2950,22 +2950,22 @@
         <v>39</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="I22" s="4" t="str">
         <f t="shared" si="0"/>
@@ -2977,22 +2977,22 @@
         <v>11</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I23" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3004,22 +3004,22 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>112</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="H24" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="I24" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3031,22 +3031,22 @@
         <v>11</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I25" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3058,22 +3058,22 @@
         <v>11</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="I26" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3085,22 +3085,22 @@
         <v>11</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="I27" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3112,22 +3112,22 @@
         <v>39</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="I28" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3139,22 +3139,22 @@
         <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D29" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="I29" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3166,22 +3166,22 @@
         <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="H30" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="I30" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3193,22 +3193,22 @@
         <v>11</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="I31" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3220,22 +3220,22 @@
         <v>11</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="I32" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3244,25 +3244,25 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="I33" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3274,22 +3274,22 @@
         <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>168</v>
-      </c>
       <c r="H34" s="2" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I34" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3301,22 +3301,22 @@
         <v>11</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="I35" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3328,22 +3328,22 @@
         <v>11</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="I36" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3355,22 +3355,22 @@
         <v>11</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="I37" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3382,22 +3382,22 @@
         <v>11</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="I38" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3406,25 +3406,25 @@
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>192</v>
-      </c>
       <c r="H39" s="2" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="I39" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3433,25 +3433,25 @@
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="G40" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="H40" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>199</v>
       </c>
       <c r="I40" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3460,25 +3460,25 @@
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I41" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3487,25 +3487,25 @@
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C42" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="G42" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D42" s="1" t="s">
+      <c r="H42" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>205</v>
       </c>
       <c r="I42" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3514,25 +3514,25 @@
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I43" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3541,25 +3541,25 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="I44" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3571,22 +3571,22 @@
         <v>11</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="I45" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3598,22 +3598,22 @@
         <v>11</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="I46" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3625,22 +3625,22 @@
         <v>11</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="I47" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3652,22 +3652,22 @@
         <v>11</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="I48" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3679,22 +3679,22 @@
         <v>11</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="I49" s="4" t="str">
         <f t="shared" si="0"/>
@@ -3706,22 +3706,22 @@
         <v>11</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="E50" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>252</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>256</v>
       </c>
       <c r="I50" s="4" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
still working on history card styling and bug fixes
</commit_message>
<xml_diff>
--- a/src/scripts/CodeBlocks/code blocks.xlsx
+++ b/src/scripts/CodeBlocks/code blocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin of the Lake\workspace\Repos\FrontEndCapstone\src\scripts\CodeBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D00E843-CF1D-4804-9214-EBF04E4DBEB9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83958B2A-70B7-45E1-A968-1ED13229F1B2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="9285" xr2:uid="{CB3B7D12-EE88-4088-ADA6-0AA53F93C8FE}"/>
   </bookViews>
@@ -2362,14 +2362,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Revert "Revert "Em enhancements""
</commit_message>
<xml_diff>
--- a/src/scripts/CodeBlocks/code blocks.xlsx
+++ b/src/scripts/CodeBlocks/code blocks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin of the Lake\workspace\Repos\FrontEndCapstone\src\scripts\CodeBlocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D00E843-CF1D-4804-9214-EBF04E4DBEB9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83958B2A-70B7-45E1-A968-1ED13229F1B2}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="9285" xr2:uid="{CB3B7D12-EE88-4088-ADA6-0AA53F93C8FE}"/>
   </bookViews>
@@ -2362,14 +2362,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H8" sqref="H8"/>
+      <selection pane="bottomLeft" activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="1" bestFit="1" customWidth="1"/>

</xml_diff>